<commit_message>
Ensuring subsetting works for x-lings
</commit_message>
<xml_diff>
--- a/inst/data/Betting.xlsx
+++ b/inst/data/Betting.xlsx
@@ -3,16 +3,16 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25318"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F67F1DF2-4748-4A87-8553-121EA3CAB21B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09B81ACF-D7C2-41A6-B722-95588F77054C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Odds" sheetId="1" r:id="rId1"/>
-    <sheet name="Overblik" sheetId="2" r:id="rId2"/>
+    <sheet name="Om dataindsamling" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Odds!$A$1:$K$149</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Odds!$A$1:$K$1</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="746" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="812" uniqueCount="227">
   <si>
     <t>BetDay</t>
   </si>
@@ -72,7 +72,7 @@
     <t>Oddset</t>
   </si>
   <si>
-    <t>Double ID 9</t>
+    <t>Double ID 9.</t>
   </si>
   <si>
     <t>Double</t>
@@ -81,7 +81,7 @@
     <t>Liverpool - Wolverhampton</t>
   </si>
   <si>
-    <t>Double ID 9: '1</t>
+    <t>Double ID 9. : '1</t>
   </si>
   <si>
     <t>Kampvinder</t>
@@ -90,7 +90,7 @@
     <t>Manchester C - Aston Villa</t>
   </si>
   <si>
-    <t>Double ID 9: Dobbeltchance Manchester C eller Uafgjort</t>
+    <t>Double ID 9. : Dobbeltchance Manchester C eller Uafgjort</t>
   </si>
   <si>
     <t>Dobbeltchance</t>
@@ -99,10 +99,10 @@
     <t>Leicester - Southampton</t>
   </si>
   <si>
-    <t>6-ling ID 8: Dobbeltchance Leicester eller Uafgjort</t>
-  </si>
-  <si>
-    <t>6-ling ID 8: '1</t>
+    <t>6-ling ID 8. : Dobbeltchance Leicester eller Uafgjort</t>
+  </si>
+  <si>
+    <t>6-ling ID 8. : '1</t>
   </si>
   <si>
     <t>Chelsea - Watford</t>
@@ -111,16 +111,16 @@
     <t>Brighton - West Ham</t>
   </si>
   <si>
-    <t>6-ling ID 8: Dobbeltchance Uafgjort eller West Ham</t>
+    <t>6-ling ID 8. : Dobbeltchance Uafgjort eller West Ham</t>
   </si>
   <si>
     <t>Norwich - Tottenham</t>
   </si>
   <si>
-    <t>6-ling ID 8: Dobbeltchance Uafgjort eller Tottenham</t>
-  </si>
-  <si>
-    <t>6-ling ID 8</t>
+    <t>6-ling ID 8. : Dobbeltchance Uafgjort eller Tottenham</t>
+  </si>
+  <si>
+    <t>6-ling ID 8.</t>
   </si>
   <si>
     <t>6-ling</t>
@@ -162,31 +162,31 @@
     <t>Dobbeltchance Uafgjort eller Manchester C</t>
   </si>
   <si>
-    <t>4-ling ID 7</t>
+    <t>4-ling ID 7.</t>
   </si>
   <si>
     <t>4-ling</t>
   </si>
   <si>
-    <t>4-ling ID 7: Dobbeltchance Uafgjort eller Manchester C</t>
+    <t>4-ling ID 7. : Dobbeltchance Uafgjort eller Manchester C</t>
   </si>
   <si>
     <t>Watford - Everton</t>
   </si>
   <si>
-    <t>4-ling ID 7: Dobbeltchance Uafgjort eller Everton</t>
+    <t>4-ling ID 7. : Dobbeltchance Uafgjort eller Everton</t>
   </si>
   <si>
     <t>Leicester - Norwich</t>
   </si>
   <si>
-    <t>4-ling ID 7: Dobbeltchance Leicester eller Uafgjort</t>
+    <t>4-ling ID 7. : Dobbeltchance Leicester eller Uafgjort</t>
   </si>
   <si>
     <t>Leeds - Chelsea</t>
   </si>
   <si>
-    <t>4-ling ID 7: Dobbeltchance Uafgjort eller Chelsea</t>
+    <t>4-ling ID 7. : Dobbeltchance Uafgjort eller Chelsea</t>
   </si>
   <si>
     <t>Aston Villa - Liverpool</t>
@@ -204,22 +204,22 @@
     <t>Manchester C - Newcastle</t>
   </si>
   <si>
-    <t>Trippel ID 6: Dobbeltchance Manchester C eller Uafgjort</t>
+    <t>Trippel ID 6. : Dobbeltchance Manchester C eller Uafgjort</t>
   </si>
   <si>
     <t>Arsenal - Leeds</t>
   </si>
   <si>
-    <t>Trippel ID 6: Dobbeltchance Arsenal eller Uafgjort</t>
+    <t>Trippel ID 6. : Dobbeltchance Arsenal eller Uafgjort</t>
   </si>
   <si>
     <t>Norwich - West Ham</t>
   </si>
   <si>
-    <t>Trippel ID 6: Dobbeltchance Uafgjort eller West Ham</t>
-  </si>
-  <si>
-    <t>Trippel ID 6</t>
+    <t>Trippel ID 6. : Dobbeltchance Uafgjort eller West Ham</t>
+  </si>
+  <si>
+    <t>Trippel ID 6.</t>
   </si>
   <si>
     <t>Trippel</t>
@@ -336,7 +336,7 @@
     <t>Hvilket hold scorer 3. mål: Manchester C</t>
   </si>
   <si>
-    <t>4-ling ID 5</t>
+    <t>4-ling ID 5.</t>
   </si>
   <si>
     <t>Arsenal - Manchester U</t>
@@ -360,7 +360,7 @@
     <t>Newcastle - Crystal P</t>
   </si>
   <si>
-    <t>Trippel ID 4: 1</t>
+    <t>Trippel ID 4. : 1</t>
   </si>
   <si>
     <t>Chelsea - Arsenal</t>
@@ -372,10 +372,10 @@
     <t>Everton - Leicester</t>
   </si>
   <si>
-    <t>Trippel ID 4: X</t>
-  </si>
-  <si>
-    <t>Trippel ID 4</t>
+    <t>Trippel ID 4. : X</t>
+  </si>
+  <si>
+    <t>Trippel ID 4.</t>
   </si>
   <si>
     <t>Liverpool - Manchester U</t>
@@ -402,16 +402,16 @@
     <t>Manchester C - Atletico Madrid</t>
   </si>
   <si>
-    <t>Double ID 3: 1</t>
+    <t>Double ID 3. : 1</t>
   </si>
   <si>
     <t>Benfica - Liverpool</t>
   </si>
   <si>
-    <t>Double ID 3: 2</t>
-  </si>
-  <si>
-    <t>Double ID 3</t>
+    <t>Double ID 3. : 2</t>
+  </si>
+  <si>
+    <t>Double ID 3.</t>
   </si>
   <si>
     <t>Nottingham F - Liverpool</t>
@@ -459,7 +459,61 @@
     <t>1 (Handicap 0 - 1)</t>
   </si>
   <si>
-    <t>13-ling ID 2</t>
+    <t>13-ling ID 2.</t>
+  </si>
+  <si>
+    <t>13-ling</t>
+  </si>
+  <si>
+    <t>Watford - Crystal P</t>
+  </si>
+  <si>
+    <t>13-ling ID 2. : 1</t>
+  </si>
+  <si>
+    <t>Brentford - Newcastle</t>
+  </si>
+  <si>
+    <t>13-ling ID 2. : X</t>
+  </si>
+  <si>
+    <t>13-ling ID 2. : Handicap (1-0) Manchester C</t>
+  </si>
+  <si>
+    <t>West Ham - Wolverhampton</t>
+  </si>
+  <si>
+    <t>Burnley - Leicester</t>
+  </si>
+  <si>
+    <t>Burnley - Tottenham</t>
+  </si>
+  <si>
+    <t>13-ling ID 2. : Handicap (0-1) Liverpool</t>
+  </si>
+  <si>
+    <t>Arsenal - Wolverhampton</t>
+  </si>
+  <si>
+    <t>13-ling ID 2. : 2</t>
+  </si>
+  <si>
+    <t>Southampton - Norwich</t>
+  </si>
+  <si>
+    <t>Leeds - Tottenham</t>
+  </si>
+  <si>
+    <t>Manchester U - Watford</t>
+  </si>
+  <si>
+    <t>13-ling ID 2. : Handicap (0-1) Manchester U</t>
+  </si>
+  <si>
+    <t>Crystal P - Burnley</t>
+  </si>
+  <si>
+    <t>Brighton - Aston Villa</t>
   </si>
   <si>
     <t>Liverpool - Norwich</t>
@@ -486,13 +540,13 @@
     <t>Manchester U - Liverpool</t>
   </si>
   <si>
-    <t>4-ling ID 1</t>
+    <t>4-ling ID 1.</t>
   </si>
   <si>
     <t>Wolverhampton - Newcastle</t>
   </si>
   <si>
-    <t>4-ling ID 1: X</t>
+    <t>4-ling ID 1. : X</t>
   </si>
   <si>
     <t>Burnley - Norwich</t>
@@ -501,7 +555,7 @@
     <t>Chelsea - Southampton</t>
   </si>
   <si>
-    <t>4-ling ID 1: 1</t>
+    <t>4-ling ID 1. : 1</t>
   </si>
   <si>
     <t>Leeds - Watford</t>
@@ -645,16 +699,19 @@
     <t>Pengene tilbage ved uafgjort: Manchester U</t>
   </si>
   <si>
-    <t>Total gevinst</t>
-  </si>
-  <si>
-    <t>Total indsats</t>
-  </si>
-  <si>
-    <t>Overskud</t>
-  </si>
-  <si>
-    <t>Afkast</t>
+    <t>Double, Tripler og x-lings:</t>
+  </si>
+  <si>
+    <t>Afsluttes med ID x.</t>
+  </si>
+  <si>
+    <t>Eksempler:</t>
+  </si>
+  <si>
+    <t>Double ID 1.</t>
+  </si>
+  <si>
+    <t>Double ID 1. : event</t>
   </si>
 </sst>
 </file>
@@ -703,12 +760,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
   </cellXfs>
@@ -1025,11 +1081,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K149"/>
+  <dimension ref="A1:K162"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
+      <pane ySplit="1" topLeftCell="A84" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B101" sqref="B101"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2097,7 +2153,7 @@
       <c r="E31" t="s">
         <v>32</v>
       </c>
-      <c r="F31" s="6" t="s">
+      <c r="F31" s="5" t="s">
         <v>66</v>
       </c>
       <c r="G31">
@@ -2217,7 +2273,7 @@
       <c r="J34">
         <v>43</v>
       </c>
-      <c r="K34" s="5" t="s">
+      <c r="K34" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2322,7 +2378,7 @@
       <c r="J37">
         <v>0</v>
       </c>
-      <c r="K37" s="5" t="s">
+      <c r="K37" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2357,7 +2413,7 @@
       <c r="J38">
         <v>10.5</v>
       </c>
-      <c r="K38" s="5" t="s">
+      <c r="K38" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -2742,7 +2798,7 @@
       <c r="J49">
         <v>66</v>
       </c>
-      <c r="K49" s="5" t="s">
+      <c r="K49" s="4" t="s">
         <v>20</v>
       </c>
     </row>
@@ -4072,350 +4128,348 @@
         <v>0</v>
       </c>
       <c r="K87" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="88" spans="1:11">
       <c r="A88" s="1">
-        <v>44611</v>
+        <v>44613</v>
       </c>
       <c r="B88" s="1">
-        <v>44611</v>
+        <v>44615</v>
       </c>
       <c r="C88" t="s">
         <v>11</v>
       </c>
       <c r="D88" t="s">
+        <v>144</v>
+      </c>
+      <c r="E88" t="s">
+        <v>12</v>
+      </c>
+      <c r="F88" t="s">
+        <v>145</v>
+      </c>
+      <c r="G88">
+        <v>3.05</v>
+      </c>
+      <c r="H88">
+        <v>0</v>
+      </c>
+      <c r="I88">
+        <v>0</v>
+      </c>
+      <c r="J88">
+        <v>0</v>
+      </c>
+      <c r="K88" t="s">
         <v>143</v>
-      </c>
-      <c r="E88" t="s">
-        <v>12</v>
-      </c>
-      <c r="F88" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G88">
-        <v>1.1299999999999999</v>
-      </c>
-      <c r="H88">
-        <v>1</v>
-      </c>
-      <c r="I88">
-        <v>95.5</v>
-      </c>
-      <c r="J88">
-        <f>G88 * I88</f>
-        <v>107.91499999999999</v>
-      </c>
-      <c r="K88" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="89" spans="1:11">
       <c r="A89" s="1">
-        <v>44608</v>
+        <v>44613</v>
       </c>
       <c r="B89" s="1">
-        <v>44608</v>
+        <v>44618</v>
       </c>
       <c r="C89" t="s">
-        <v>70</v>
+        <v>11</v>
       </c>
       <c r="D89" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="E89" t="s">
         <v>12</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>53</v>
+      <c r="F89" t="s">
+        <v>147</v>
       </c>
       <c r="G89">
-        <v>2.25</v>
+        <v>3.4</v>
       </c>
       <c r="H89">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I89">
-        <v>42.5</v>
+        <v>0</v>
       </c>
       <c r="J89">
-        <f>IF(H89 = 1, G89 * I89, 0)</f>
-        <v>95.625</v>
+        <v>0</v>
       </c>
       <c r="K89" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="90" spans="1:11">
       <c r="A90" s="1">
-        <v>44584</v>
+        <v>44613</v>
       </c>
       <c r="B90" s="1">
-        <v>44584</v>
+        <v>44618</v>
       </c>
       <c r="C90" t="s">
         <v>11</v>
       </c>
       <c r="D90" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="E90" t="s">
         <v>12</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>53</v>
+      <c r="F90" t="s">
+        <v>148</v>
       </c>
       <c r="G90">
-        <v>1.58</v>
+        <v>1.75</v>
       </c>
       <c r="H90">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I90">
-        <v>27.03</v>
+        <v>0</v>
       </c>
       <c r="J90">
-        <f>IF(H90 = 1, G90 * I90, 0)</f>
-        <v>42.707400000000007</v>
+        <v>0</v>
       </c>
       <c r="K90" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="91" spans="1:11">
       <c r="A91" s="1">
-        <v>44558</v>
+        <v>44613</v>
       </c>
       <c r="B91" s="1">
-        <v>44558</v>
+        <v>44619</v>
       </c>
       <c r="C91" t="s">
         <v>11</v>
       </c>
       <c r="D91" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="E91" t="s">
-        <v>32</v>
-      </c>
-      <c r="F91" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
+      </c>
+      <c r="F91" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G91">
-        <v>1.34</v>
+        <v>3.4</v>
       </c>
       <c r="H91">
         <v>0</v>
       </c>
       <c r="I91">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J91">
         <v>0</v>
       </c>
       <c r="K91" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="92" spans="1:11">
       <c r="A92" s="1">
-        <v>44541</v>
+        <v>44613</v>
       </c>
       <c r="B92" s="1">
-        <v>44541</v>
+        <v>44621</v>
       </c>
       <c r="C92" t="s">
         <v>11</v>
       </c>
       <c r="D92" t="s">
+        <v>150</v>
+      </c>
+      <c r="E92" t="s">
+        <v>12</v>
+      </c>
+      <c r="F92" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="E92" t="s">
-        <v>32</v>
-      </c>
-      <c r="F92" s="3" t="s">
-        <v>141</v>
-      </c>
       <c r="G92">
-        <v>1.7</v>
+        <v>3.65</v>
       </c>
       <c r="H92">
         <v>0</v>
       </c>
       <c r="I92">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J92">
         <v>0</v>
       </c>
       <c r="K92" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="93" spans="1:11">
       <c r="A93" s="1">
-        <v>44534</v>
+        <v>44613</v>
       </c>
       <c r="B93" s="1">
-        <v>44534</v>
+        <v>44615</v>
       </c>
       <c r="C93" t="s">
         <v>11</v>
       </c>
       <c r="D93" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="E93" t="s">
-        <v>32</v>
-      </c>
-      <c r="F93" t="s">
-        <v>97</v>
+        <v>12</v>
+      </c>
+      <c r="F93" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G93">
-        <v>3.2</v>
+        <v>3.65</v>
       </c>
       <c r="H93">
         <v>0</v>
       </c>
       <c r="I93">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J93">
         <v>0</v>
       </c>
       <c r="K93" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="94" spans="1:11">
       <c r="A94" s="1">
-        <v>44531</v>
+        <v>44613</v>
       </c>
       <c r="B94" s="1">
-        <v>44531</v>
+        <v>44615</v>
       </c>
       <c r="C94" t="s">
         <v>11</v>
       </c>
       <c r="D94" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E94" t="s">
-        <v>32</v>
-      </c>
-      <c r="F94" s="3" t="s">
-        <v>53</v>
+        <v>12</v>
+      </c>
+      <c r="F94" s="2" t="s">
+        <v>152</v>
       </c>
       <c r="G94">
-        <v>1.37</v>
+        <v>1.42</v>
       </c>
       <c r="H94">
         <v>1</v>
       </c>
       <c r="I94">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J94">
-        <f>G94 * I94</f>
-        <v>137</v>
+        <v>0</v>
       </c>
       <c r="K94" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="95" spans="1:11">
       <c r="A95" s="1">
-        <v>44493</v>
+        <v>44613</v>
       </c>
       <c r="B95" s="1">
-        <v>44493</v>
+        <v>44594</v>
       </c>
       <c r="C95" t="s">
         <v>11</v>
       </c>
       <c r="D95" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="E95" t="s">
         <v>12</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>53</v>
+      <c r="F95" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="G95">
-        <v>2.4500000000000002</v>
+        <v>5.7</v>
       </c>
       <c r="H95">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I95">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J95">
-        <f>G95 * I95</f>
-        <v>122.50000000000001</v>
+        <v>0</v>
       </c>
       <c r="K95" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="96" spans="1:11">
       <c r="A96" s="1">
-        <v>44471</v>
+        <v>44613</v>
       </c>
       <c r="B96" s="1">
-        <v>44471</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>11</v>
+        <v>44594</v>
+      </c>
+      <c r="C96" t="s">
+        <v>11</v>
+      </c>
+      <c r="D96" t="s">
+        <v>155</v>
       </c>
       <c r="E96" t="s">
-        <v>32</v>
-      </c>
-      <c r="F96" t="s">
-        <v>151</v>
+        <v>12</v>
+      </c>
+      <c r="F96" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G96">
-        <v>8.4700000000000006</v>
+        <v>4.2</v>
       </c>
       <c r="H96">
         <v>0</v>
       </c>
       <c r="I96">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J96">
         <v>0</v>
       </c>
       <c r="K96" t="s">
-        <v>44</v>
+        <v>143</v>
       </c>
     </row>
     <row r="97" spans="1:11">
       <c r="A97" s="1">
-        <v>44471</v>
+        <v>44613</v>
       </c>
       <c r="B97" s="1">
-        <v>44471</v>
-      </c>
-      <c r="C97" s="2" t="s">
+        <v>44618</v>
+      </c>
+      <c r="C97" t="s">
         <v>11</v>
       </c>
       <c r="D97" t="s">
-        <v>152</v>
+        <v>156</v>
       </c>
       <c r="E97" t="s">
-        <v>32</v>
-      </c>
-      <c r="F97" t="s">
-        <v>153</v>
+        <v>12</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>154</v>
       </c>
       <c r="G97">
-        <v>2.4500000000000002</v>
+        <v>2</v>
       </c>
       <c r="H97">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I97">
         <v>0</v>
@@ -4424,33 +4478,33 @@
         <v>0</v>
       </c>
       <c r="K97" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="98" spans="1:11">
       <c r="A98" s="1">
-        <v>44471</v>
+        <v>44613</v>
       </c>
       <c r="B98" s="1">
-        <v>44471</v>
-      </c>
-      <c r="C98" s="2" t="s">
+        <v>44618</v>
+      </c>
+      <c r="C98" t="s">
         <v>11</v>
       </c>
       <c r="D98" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="E98" t="s">
-        <v>32</v>
-      </c>
-      <c r="F98" t="s">
-        <v>153</v>
+        <v>12</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>158</v>
       </c>
       <c r="G98">
-        <v>2.5499999999999998</v>
+        <v>1.92</v>
       </c>
       <c r="H98">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I98">
         <v>0</v>
@@ -4459,30 +4513,30 @@
         <v>0</v>
       </c>
       <c r="K98" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="99" spans="1:11">
       <c r="A99" s="1">
-        <v>44471</v>
+        <v>44613</v>
       </c>
       <c r="B99" s="1">
-        <v>44471</v>
-      </c>
-      <c r="C99" s="2" t="s">
+        <v>44618</v>
+      </c>
+      <c r="C99" t="s">
         <v>11</v>
       </c>
       <c r="D99" t="s">
-        <v>155</v>
+        <v>159</v>
       </c>
       <c r="E99" t="s">
-        <v>32</v>
-      </c>
-      <c r="F99" s="3" t="s">
-        <v>156</v>
+        <v>12</v>
+      </c>
+      <c r="F99" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G99">
-        <v>1.1499999999999999</v>
+        <v>3.55</v>
       </c>
       <c r="H99">
         <v>1</v>
@@ -4494,33 +4548,33 @@
         <v>0</v>
       </c>
       <c r="K99" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="100" spans="1:11">
       <c r="A100" s="1">
-        <v>44471</v>
+        <v>44613</v>
       </c>
       <c r="B100" s="1">
-        <v>44471</v>
-      </c>
-      <c r="C100" s="2" t="s">
+        <v>44618</v>
+      </c>
+      <c r="C100" t="s">
         <v>11</v>
       </c>
       <c r="D100" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="E100" t="s">
-        <v>32</v>
-      </c>
-      <c r="F100" t="s">
-        <v>156</v>
+        <v>12</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>147</v>
       </c>
       <c r="G100">
-        <v>1.18</v>
+        <v>3.25</v>
       </c>
       <c r="H100">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I100">
         <v>0</v>
@@ -4529,75 +4583,76 @@
         <v>0</v>
       </c>
       <c r="K100" t="s">
-        <v>17</v>
+        <v>143</v>
       </c>
     </row>
     <row r="101" spans="1:11">
       <c r="A101" s="1">
-        <v>44471</v>
+        <v>44611</v>
       </c>
       <c r="B101" s="1">
-        <v>44471</v>
-      </c>
-      <c r="C101" s="2" t="s">
+        <v>44611</v>
+      </c>
+      <c r="C101" t="s">
         <v>11</v>
       </c>
       <c r="D101" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="E101" t="s">
         <v>12</v>
       </c>
-      <c r="F101" t="s">
-        <v>159</v>
+      <c r="F101" s="3" t="s">
+        <v>69</v>
       </c>
       <c r="G101">
-        <v>1.3</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H101">
         <v>1</v>
       </c>
       <c r="I101">
-        <v>29</v>
+        <v>95.5</v>
       </c>
       <c r="J101">
         <f>G101 * I101</f>
-        <v>37.700000000000003</v>
+        <v>107.91499999999999</v>
       </c>
       <c r="K101" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="102" spans="1:11">
       <c r="A102" s="1">
-        <v>44464</v>
+        <v>44608</v>
       </c>
       <c r="B102" s="1">
-        <v>44464</v>
-      </c>
-      <c r="C102" s="2" t="s">
-        <v>11</v>
+        <v>44608</v>
+      </c>
+      <c r="C102" t="s">
+        <v>70</v>
       </c>
       <c r="D102" t="s">
-        <v>160</v>
-      </c>
-      <c r="E102" s="2" t="s">
-        <v>32</v>
+        <v>162</v>
+      </c>
+      <c r="E102" t="s">
+        <v>12</v>
       </c>
       <c r="F102" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G102">
-        <v>1.4</v>
+        <v>2.25</v>
       </c>
       <c r="H102">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I102">
-        <v>50</v>
+        <v>42.5</v>
       </c>
       <c r="J102">
-        <v>0</v>
+        <f>IF(H102 = 1, G102 * I102, 0)</f>
+        <v>95.625</v>
       </c>
       <c r="K102" t="s">
         <v>17</v>
@@ -4605,31 +4660,35 @@
     </row>
     <row r="103" spans="1:11">
       <c r="A103" s="1">
-        <v>44464</v>
+        <v>44584</v>
       </c>
       <c r="B103" s="1">
-        <v>44464</v>
-      </c>
-      <c r="C103" s="2" t="s">
+        <v>44584</v>
+      </c>
+      <c r="C103" t="s">
         <v>11</v>
       </c>
       <c r="D103" t="s">
-        <v>161</v>
-      </c>
-      <c r="E103" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F103" t="s">
-        <v>106</v>
+        <v>163</v>
+      </c>
+      <c r="E103" t="s">
+        <v>12</v>
+      </c>
+      <c r="F103" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G103">
-        <v>1.62</v>
+        <v>1.58</v>
       </c>
       <c r="H103">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I103">
-        <v>10</v>
+        <v>27.03</v>
+      </c>
+      <c r="J103">
+        <f>IF(H103 = 1, G103 * I103, 0)</f>
+        <v>42.707400000000007</v>
       </c>
       <c r="K103" t="s">
         <v>17</v>
@@ -4637,60 +4696,60 @@
     </row>
     <row r="104" spans="1:11">
       <c r="A104" s="1">
-        <v>44464</v>
+        <v>44558</v>
       </c>
       <c r="B104" s="1">
-        <v>44464</v>
-      </c>
-      <c r="C104" s="2" t="s">
+        <v>44558</v>
+      </c>
+      <c r="C104" t="s">
         <v>11</v>
       </c>
       <c r="D104" t="s">
-        <v>162</v>
-      </c>
-      <c r="E104" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F104" t="s">
-        <v>163</v>
+        <v>164</v>
+      </c>
+      <c r="E104" t="s">
+        <v>32</v>
+      </c>
+      <c r="F104" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G104">
-        <v>8.5</v>
+        <v>1.34</v>
       </c>
       <c r="H104">
         <v>0</v>
       </c>
       <c r="I104">
-        <v>10</v>
+        <v>50</v>
       </c>
       <c r="J104">
         <v>0</v>
       </c>
       <c r="K104" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="105" spans="1:11">
       <c r="A105" s="1">
-        <v>44454</v>
+        <v>44541</v>
       </c>
       <c r="B105" s="1">
-        <v>44454</v>
-      </c>
-      <c r="C105" s="2" t="s">
-        <v>70</v>
+        <v>44541</v>
+      </c>
+      <c r="C105" t="s">
+        <v>11</v>
       </c>
       <c r="D105" t="s">
-        <v>164</v>
-      </c>
-      <c r="E105" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F105" t="s">
-        <v>131</v>
+        <v>165</v>
+      </c>
+      <c r="E105" t="s">
+        <v>32</v>
+      </c>
+      <c r="F105" s="3" t="s">
+        <v>141</v>
       </c>
       <c r="G105">
-        <v>1.45</v>
+        <v>1.7</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -4702,40 +4761,39 @@
         <v>0</v>
       </c>
       <c r="K105" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="106" spans="1:11">
       <c r="A106" s="1">
-        <v>44454</v>
+        <v>44534</v>
       </c>
       <c r="B106" s="1">
-        <v>44454</v>
-      </c>
-      <c r="C106" s="2" t="s">
-        <v>70</v>
+        <v>44534</v>
+      </c>
+      <c r="C106" t="s">
+        <v>11</v>
       </c>
       <c r="D106" t="s">
-        <v>164</v>
-      </c>
-      <c r="E106" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F106" s="3" t="s">
-        <v>69</v>
+        <v>166</v>
+      </c>
+      <c r="E106" t="s">
+        <v>32</v>
+      </c>
+      <c r="F106" t="s">
+        <v>97</v>
       </c>
       <c r="G106">
-        <v>1.43</v>
+        <v>3.2</v>
       </c>
       <c r="H106">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I106">
-        <v>34</v>
+        <v>50</v>
       </c>
       <c r="J106">
-        <f>G106 * I106</f>
-        <v>48.62</v>
+        <v>0</v>
       </c>
       <c r="K106" t="s">
         <v>17</v>
@@ -4743,34 +4801,35 @@
     </row>
     <row r="107" spans="1:11">
       <c r="A107" s="1">
-        <v>44453</v>
+        <v>44531</v>
       </c>
       <c r="B107" s="1">
-        <v>44453</v>
-      </c>
-      <c r="C107" s="2" t="s">
-        <v>70</v>
+        <v>44531</v>
+      </c>
+      <c r="C107" t="s">
+        <v>11</v>
       </c>
       <c r="D107" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="E107" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="F107" s="3" t="s">
         <v>53</v>
       </c>
       <c r="G107">
-        <v>1.42</v>
+        <v>1.37</v>
       </c>
       <c r="H107">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I107">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J107">
-        <v>0</v>
+        <f>G107 * I107</f>
+        <v>137</v>
       </c>
       <c r="K107" t="s">
         <v>17</v>
@@ -4778,25 +4837,25 @@
     </row>
     <row r="108" spans="1:11">
       <c r="A108" s="1">
-        <v>44451</v>
+        <v>44493</v>
       </c>
       <c r="B108" s="1">
-        <v>44451</v>
-      </c>
-      <c r="C108" s="2" t="s">
+        <v>44493</v>
+      </c>
+      <c r="C108" t="s">
         <v>11</v>
       </c>
       <c r="D108" t="s">
-        <v>166</v>
-      </c>
-      <c r="E108" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F108" t="s">
-        <v>167</v>
+        <v>168</v>
+      </c>
+      <c r="E108" t="s">
+        <v>12</v>
+      </c>
+      <c r="F108" s="3" t="s">
+        <v>53</v>
       </c>
       <c r="G108">
-        <v>1.35</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H108">
         <v>1</v>
@@ -4806,74 +4865,71 @@
       </c>
       <c r="J108">
         <f>G108 * I108</f>
-        <v>67.5</v>
+        <v>122.50000000000001</v>
       </c>
       <c r="K108" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="109" spans="1:11">
       <c r="A109" s="1">
-        <v>44450</v>
+        <v>44471</v>
       </c>
       <c r="B109" s="1">
-        <v>44450</v>
+        <v>44471</v>
       </c>
       <c r="C109" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D109" t="s">
-        <v>168</v>
-      </c>
-      <c r="E109" s="2" t="s">
+      <c r="E109" t="s">
         <v>32</v>
       </c>
       <c r="F109" t="s">
         <v>169</v>
       </c>
       <c r="G109">
-        <v>1.42</v>
+        <v>8.4700000000000006</v>
       </c>
       <c r="H109">
         <v>0</v>
       </c>
       <c r="I109">
-        <v>100</v>
+        <v>10</v>
       </c>
       <c r="J109">
         <v>0</v>
       </c>
       <c r="K109" t="s">
-        <v>34</v>
+        <v>44</v>
       </c>
     </row>
     <row r="110" spans="1:11">
       <c r="A110" s="1">
-        <v>44450</v>
+        <v>44471</v>
       </c>
       <c r="B110" s="1">
-        <v>44450</v>
+        <v>44471</v>
       </c>
       <c r="C110" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D110" t="s">
-        <v>168</v>
-      </c>
-      <c r="E110" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="E110" t="s">
         <v>32</v>
       </c>
       <c r="F110" t="s">
-        <v>87</v>
+        <v>171</v>
       </c>
       <c r="G110">
-        <v>1.28</v>
+        <v>2.4500000000000002</v>
       </c>
       <c r="H110">
         <v>0</v>
       </c>
       <c r="I110">
-        <v>50</v>
+        <v>0</v>
       </c>
       <c r="J110">
         <v>0</v>
@@ -4884,141 +4940,140 @@
     </row>
     <row r="111" spans="1:11">
       <c r="A111" s="1">
-        <v>44450</v>
+        <v>44471</v>
       </c>
       <c r="B111" s="1">
-        <v>44450</v>
+        <v>44471</v>
       </c>
       <c r="C111" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D111" t="s">
-        <v>168</v>
-      </c>
-      <c r="E111" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="E111" t="s">
         <v>32</v>
       </c>
       <c r="F111" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="G111">
-        <v>1.5</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="H111">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I111">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J111">
         <v>0</v>
       </c>
       <c r="K111" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="112" spans="1:11">
       <c r="A112" s="1">
-        <v>44437</v>
+        <v>44471</v>
       </c>
       <c r="B112" s="1">
-        <v>44437</v>
+        <v>44471</v>
       </c>
       <c r="C112" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D112" t="s">
-        <v>171</v>
-      </c>
-      <c r="E112" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F112" t="s">
-        <v>172</v>
+        <v>173</v>
+      </c>
+      <c r="E112" t="s">
+        <v>32</v>
+      </c>
+      <c r="F112" s="3" t="s">
+        <v>174</v>
       </c>
       <c r="G112">
-        <v>9.5</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H112">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I112">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="J112">
         <v>0</v>
       </c>
       <c r="K112" t="s">
-        <v>67</v>
+        <v>17</v>
       </c>
     </row>
     <row r="113" spans="1:11">
       <c r="A113" s="1">
-        <v>44436</v>
+        <v>44471</v>
       </c>
       <c r="B113" s="1">
-        <v>44436</v>
+        <v>44471</v>
       </c>
       <c r="C113" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D113" t="s">
-        <v>173</v>
-      </c>
-      <c r="E113" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E113" t="s">
         <v>32</v>
       </c>
       <c r="F113" t="s">
         <v>174</v>
       </c>
       <c r="G113">
-        <v>1.1200000000000001</v>
+        <v>1.18</v>
       </c>
       <c r="H113">
         <v>1</v>
       </c>
       <c r="I113">
-        <v>100</v>
+        <v>0</v>
       </c>
       <c r="J113">
-        <f>G113 * I113</f>
-        <v>112.00000000000001</v>
+        <v>0</v>
       </c>
       <c r="K113" t="s">
-        <v>34</v>
+        <v>17</v>
       </c>
     </row>
     <row r="114" spans="1:11">
       <c r="A114" s="1">
-        <v>44436</v>
+        <v>44471</v>
       </c>
       <c r="B114" s="1">
-        <v>44436</v>
+        <v>44471</v>
       </c>
       <c r="C114" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D114" t="s">
-        <v>173</v>
-      </c>
-      <c r="E114" s="2" t="s">
-        <v>32</v>
+        <v>176</v>
+      </c>
+      <c r="E114" t="s">
+        <v>12</v>
       </c>
       <c r="F114" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="G114">
-        <v>1.42</v>
+        <v>1.3</v>
       </c>
       <c r="H114">
         <v>1</v>
       </c>
       <c r="I114">
-        <v>50</v>
+        <v>29</v>
       </c>
       <c r="J114">
         <f>G114 * I114</f>
-        <v>71</v>
+        <v>37.700000000000003</v>
       </c>
       <c r="K114" t="s">
         <v>34</v>
@@ -5026,31 +5081,31 @@
     </row>
     <row r="115" spans="1:11">
       <c r="A115" s="1">
-        <v>44375</v>
+        <v>44464</v>
       </c>
       <c r="B115" s="1">
-        <v>44375</v>
+        <v>44464</v>
       </c>
       <c r="C115" s="2" t="s">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="D115" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="E115" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F115" s="3" t="s">
-        <v>69</v>
+        <v>53</v>
       </c>
       <c r="G115">
-        <v>1.58</v>
+        <v>1.4</v>
       </c>
       <c r="H115">
         <v>0</v>
       </c>
       <c r="I115">
-        <v>100</v>
+        <v>50</v>
       </c>
       <c r="J115">
         <v>0</v>
@@ -5061,34 +5116,31 @@
     </row>
     <row r="116" spans="1:11">
       <c r="A116" s="1">
-        <v>44374</v>
+        <v>44464</v>
       </c>
       <c r="B116" s="1">
-        <v>44374</v>
+        <v>44464</v>
       </c>
       <c r="C116" s="2" t="s">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="D116" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="E116" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F116" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="G116">
-        <v>1.82</v>
+        <v>1.62</v>
       </c>
       <c r="H116">
         <v>0</v>
       </c>
       <c r="I116">
-        <v>50</v>
-      </c>
-      <c r="J116">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="K116" t="s">
         <v>17</v>
@@ -5096,70 +5148,69 @@
     </row>
     <row r="117" spans="1:11">
       <c r="A117" s="1">
-        <v>44374</v>
+        <v>44464</v>
       </c>
       <c r="B117" s="1">
-        <v>44374</v>
+        <v>44464</v>
       </c>
       <c r="C117" s="2" t="s">
-        <v>176</v>
+        <v>11</v>
       </c>
       <c r="D117" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="E117" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F117" t="s">
-        <v>106</v>
+        <v>181</v>
       </c>
       <c r="G117">
-        <v>3.05</v>
+        <v>8.5</v>
       </c>
       <c r="H117">
         <v>0</v>
       </c>
       <c r="I117">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="J117">
         <v>0</v>
       </c>
       <c r="K117" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
     </row>
     <row r="118" spans="1:11">
       <c r="A118" s="1">
-        <v>44374</v>
+        <v>44454</v>
       </c>
       <c r="B118" s="1">
-        <v>44374</v>
+        <v>44454</v>
       </c>
       <c r="C118" s="2" t="s">
-        <v>176</v>
+        <v>70</v>
       </c>
       <c r="D118" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="E118" s="2" t="s">
         <v>32</v>
       </c>
       <c r="F118" t="s">
-        <v>159</v>
+        <v>131</v>
       </c>
       <c r="G118">
-        <v>1.24</v>
+        <v>1.45</v>
       </c>
       <c r="H118">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I118">
         <v>50</v>
       </c>
       <c r="J118">
-        <f t="shared" ref="J118:J120" si="0">G118 * I118</f>
-        <v>62</v>
+        <v>0</v>
       </c>
       <c r="K118" t="s">
         <v>34</v>
@@ -5167,1016 +5218,1012 @@
     </row>
     <row r="119" spans="1:11">
       <c r="A119" s="1">
+        <v>44454</v>
+      </c>
+      <c r="B119" s="1">
+        <v>44454</v>
+      </c>
+      <c r="C119" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D119" t="s">
+        <v>182</v>
+      </c>
+      <c r="E119" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F119" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G119">
+        <v>1.43</v>
+      </c>
+      <c r="H119">
+        <v>1</v>
+      </c>
+      <c r="I119">
+        <v>34</v>
+      </c>
+      <c r="J119">
+        <f>G119 * I119</f>
+        <v>48.62</v>
+      </c>
+      <c r="K119" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="120" spans="1:11">
+      <c r="A120" s="1">
+        <v>44453</v>
+      </c>
+      <c r="B120" s="1">
+        <v>44453</v>
+      </c>
+      <c r="C120" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D120" t="s">
+        <v>183</v>
+      </c>
+      <c r="E120" t="s">
+        <v>12</v>
+      </c>
+      <c r="F120" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G120">
+        <v>1.42</v>
+      </c>
+      <c r="H120">
+        <v>0</v>
+      </c>
+      <c r="I120">
+        <v>50</v>
+      </c>
+      <c r="J120">
+        <v>0</v>
+      </c>
+      <c r="K120" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="121" spans="1:11">
+      <c r="A121" s="1">
+        <v>44451</v>
+      </c>
+      <c r="B121" s="1">
+        <v>44451</v>
+      </c>
+      <c r="C121" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D121" t="s">
+        <v>184</v>
+      </c>
+      <c r="E121" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F121" t="s">
+        <v>185</v>
+      </c>
+      <c r="G121">
+        <v>1.35</v>
+      </c>
+      <c r="H121">
+        <v>1</v>
+      </c>
+      <c r="I121">
+        <v>50</v>
+      </c>
+      <c r="J121">
+        <f>G121 * I121</f>
+        <v>67.5</v>
+      </c>
+      <c r="K121" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="122" spans="1:11">
+      <c r="A122" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B122" s="1">
+        <v>44450</v>
+      </c>
+      <c r="C122" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D122" t="s">
+        <v>186</v>
+      </c>
+      <c r="E122" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F122" t="s">
+        <v>187</v>
+      </c>
+      <c r="G122">
+        <v>1.42</v>
+      </c>
+      <c r="H122">
+        <v>0</v>
+      </c>
+      <c r="I122">
+        <v>100</v>
+      </c>
+      <c r="J122">
+        <v>0</v>
+      </c>
+      <c r="K122" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="123" spans="1:11">
+      <c r="A123" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B123" s="1">
+        <v>44450</v>
+      </c>
+      <c r="C123" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D123" t="s">
+        <v>186</v>
+      </c>
+      <c r="E123" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F123" t="s">
+        <v>87</v>
+      </c>
+      <c r="G123">
+        <v>1.28</v>
+      </c>
+      <c r="H123">
+        <v>0</v>
+      </c>
+      <c r="I123">
+        <v>50</v>
+      </c>
+      <c r="J123">
+        <v>0</v>
+      </c>
+      <c r="K123" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="124" spans="1:11">
+      <c r="A124" s="1">
+        <v>44450</v>
+      </c>
+      <c r="B124" s="1">
+        <v>44450</v>
+      </c>
+      <c r="C124" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D124" t="s">
+        <v>186</v>
+      </c>
+      <c r="E124" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F124" t="s">
+        <v>188</v>
+      </c>
+      <c r="G124">
+        <v>1.5</v>
+      </c>
+      <c r="H124">
+        <v>0</v>
+      </c>
+      <c r="I124">
+        <v>100</v>
+      </c>
+      <c r="J124">
+        <v>0</v>
+      </c>
+      <c r="K124" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="125" spans="1:11">
+      <c r="A125" s="1">
+        <v>44437</v>
+      </c>
+      <c r="B125" s="1">
+        <v>44437</v>
+      </c>
+      <c r="C125" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D125" t="s">
+        <v>189</v>
+      </c>
+      <c r="E125" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F125" t="s">
+        <v>190</v>
+      </c>
+      <c r="G125">
+        <v>9.5</v>
+      </c>
+      <c r="H125">
+        <v>0</v>
+      </c>
+      <c r="I125">
+        <v>10</v>
+      </c>
+      <c r="J125">
+        <v>0</v>
+      </c>
+      <c r="K125" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="126" spans="1:11">
+      <c r="A126" s="1">
+        <v>44436</v>
+      </c>
+      <c r="B126" s="1">
+        <v>44436</v>
+      </c>
+      <c r="C126" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D126" t="s">
+        <v>191</v>
+      </c>
+      <c r="E126" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F126" t="s">
+        <v>192</v>
+      </c>
+      <c r="G126">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="H126">
+        <v>1</v>
+      </c>
+      <c r="I126">
+        <v>100</v>
+      </c>
+      <c r="J126">
+        <f>G126 * I126</f>
+        <v>112.00000000000001</v>
+      </c>
+      <c r="K126" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="127" spans="1:11">
+      <c r="A127" s="1">
+        <v>44436</v>
+      </c>
+      <c r="B127" s="1">
+        <v>44436</v>
+      </c>
+      <c r="C127" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D127" t="s">
+        <v>191</v>
+      </c>
+      <c r="E127" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F127" t="s">
+        <v>193</v>
+      </c>
+      <c r="G127">
+        <v>1.42</v>
+      </c>
+      <c r="H127">
+        <v>1</v>
+      </c>
+      <c r="I127">
+        <v>50</v>
+      </c>
+      <c r="J127">
+        <f>G127 * I127</f>
+        <v>71</v>
+      </c>
+      <c r="K127" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="128" spans="1:11">
+      <c r="A128" s="1">
+        <v>44375</v>
+      </c>
+      <c r="B128" s="1">
+        <v>44375</v>
+      </c>
+      <c r="C128" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D128" t="s">
+        <v>195</v>
+      </c>
+      <c r="E128" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F128" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G128">
+        <v>1.58</v>
+      </c>
+      <c r="H128">
+        <v>0</v>
+      </c>
+      <c r="I128">
+        <v>100</v>
+      </c>
+      <c r="J128">
+        <v>0</v>
+      </c>
+      <c r="K128" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="129" spans="1:11">
+      <c r="A129" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B129" s="1">
+        <v>44374</v>
+      </c>
+      <c r="C129" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D129" t="s">
+        <v>196</v>
+      </c>
+      <c r="E129" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F129" t="s">
+        <v>87</v>
+      </c>
+      <c r="G129">
+        <v>1.82</v>
+      </c>
+      <c r="H129">
+        <v>0</v>
+      </c>
+      <c r="I129">
+        <v>50</v>
+      </c>
+      <c r="J129">
+        <v>0</v>
+      </c>
+      <c r="K129" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="130" spans="1:11">
+      <c r="A130" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B130" s="1">
+        <v>44374</v>
+      </c>
+      <c r="C130" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D130" t="s">
+        <v>196</v>
+      </c>
+      <c r="E130" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F130" t="s">
+        <v>106</v>
+      </c>
+      <c r="G130">
+        <v>3.05</v>
+      </c>
+      <c r="H130">
+        <v>0</v>
+      </c>
+      <c r="I130">
+        <v>0</v>
+      </c>
+      <c r="J130">
+        <v>0</v>
+      </c>
+      <c r="K130" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="1:11">
+      <c r="A131" s="1">
+        <v>44374</v>
+      </c>
+      <c r="B131" s="1">
+        <v>44374</v>
+      </c>
+      <c r="C131" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D131" t="s">
+        <v>196</v>
+      </c>
+      <c r="E131" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F131" t="s">
+        <v>177</v>
+      </c>
+      <c r="G131">
+        <v>1.24</v>
+      </c>
+      <c r="H131">
+        <v>1</v>
+      </c>
+      <c r="I131">
+        <v>50</v>
+      </c>
+      <c r="J131">
+        <f t="shared" ref="J131:J133" si="0">G131 * I131</f>
+        <v>62</v>
+      </c>
+      <c r="K131" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="132" spans="1:11">
+      <c r="A132" s="1">
         <v>44373</v>
       </c>
-      <c r="B119" s="1">
+      <c r="B132" s="1">
         <v>44373</v>
       </c>
-      <c r="C119" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D119" t="s">
-        <v>179</v>
-      </c>
-      <c r="E119" t="s">
-        <v>12</v>
-      </c>
-      <c r="F119" s="3" t="s">
+      <c r="C132" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D132" t="s">
+        <v>197</v>
+      </c>
+      <c r="E132" t="s">
+        <v>12</v>
+      </c>
+      <c r="F132" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G119">
+      <c r="G132">
         <v>1.92</v>
       </c>
-      <c r="H119">
-        <v>1</v>
-      </c>
-      <c r="I119">
+      <c r="H132">
+        <v>1</v>
+      </c>
+      <c r="I132">
         <v>100</v>
       </c>
-      <c r="J119">
+      <c r="J132">
         <f t="shared" si="0"/>
         <v>192</v>
       </c>
-      <c r="K119" t="s">
+      <c r="K132" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="120" spans="1:11">
-      <c r="A120" s="1">
+    <row r="133" spans="1:11">
+      <c r="A133" s="1">
         <v>44368</v>
       </c>
-      <c r="B120" s="1">
+      <c r="B133" s="1">
         <v>44368</v>
       </c>
-      <c r="C120" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D120" t="s">
-        <v>180</v>
-      </c>
-      <c r="E120" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F120" s="3" t="s">
+      <c r="C133" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D133" t="s">
+        <v>198</v>
+      </c>
+      <c r="E133" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F133" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G120">
+      <c r="G133">
         <v>1.2</v>
       </c>
-      <c r="H120">
-        <v>1</v>
-      </c>
-      <c r="I120">
+      <c r="H133">
+        <v>1</v>
+      </c>
+      <c r="I133">
         <v>200</v>
       </c>
-      <c r="J120">
+      <c r="J133">
         <f t="shared" si="0"/>
         <v>240</v>
       </c>
-      <c r="K120" t="s">
+      <c r="K133" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="121" spans="1:11">
-      <c r="A121" s="1">
+    <row r="134" spans="1:11">
+      <c r="A134" s="1">
         <v>44368</v>
       </c>
-      <c r="B121" s="1">
+      <c r="B134" s="1">
         <v>44368</v>
       </c>
-      <c r="C121" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D121" t="s">
-        <v>180</v>
-      </c>
-      <c r="E121" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F121" t="s">
-        <v>181</v>
-      </c>
-      <c r="G121">
+      <c r="C134" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D134" t="s">
+        <v>198</v>
+      </c>
+      <c r="E134" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F134" t="s">
+        <v>199</v>
+      </c>
+      <c r="G134">
         <v>1.42</v>
       </c>
-      <c r="H121">
-        <v>0</v>
-      </c>
-      <c r="I121">
+      <c r="H134">
+        <v>0</v>
+      </c>
+      <c r="I134">
         <v>100</v>
       </c>
-      <c r="J121">
-        <v>0</v>
-      </c>
-      <c r="K121" t="s">
+      <c r="J134">
+        <v>0</v>
+      </c>
+      <c r="K134" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="122" spans="1:11">
-      <c r="A122" s="1">
+    <row r="135" spans="1:11">
+      <c r="A135" s="1">
         <v>44368</v>
       </c>
-      <c r="B122" s="1">
+      <c r="B135" s="1">
         <v>44368</v>
       </c>
-      <c r="C122" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D122" t="s">
-        <v>180</v>
-      </c>
-      <c r="E122" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F122" t="s">
-        <v>182</v>
-      </c>
-      <c r="G122">
+      <c r="C135" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D135" t="s">
+        <v>198</v>
+      </c>
+      <c r="E135" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F135" t="s">
+        <v>200</v>
+      </c>
+      <c r="G135">
         <v>1.1299999999999999</v>
       </c>
-      <c r="H122">
-        <v>1</v>
-      </c>
-      <c r="I122">
+      <c r="H135">
+        <v>1</v>
+      </c>
+      <c r="I135">
         <v>100</v>
       </c>
-      <c r="J122">
-        <f t="shared" ref="J122:J123" si="1">G122 * I122</f>
+      <c r="J135">
+        <f t="shared" ref="J135:J136" si="1">G135 * I135</f>
         <v>112.99999999999999</v>
       </c>
-      <c r="K122" t="s">
+      <c r="K135" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="123" spans="1:11">
-      <c r="A123" s="1">
+    <row r="136" spans="1:11">
+      <c r="A136" s="1">
         <v>44368</v>
       </c>
-      <c r="B123" s="1">
+      <c r="B136" s="1">
         <v>44368</v>
       </c>
-      <c r="C123" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D123" t="s">
-        <v>180</v>
-      </c>
-      <c r="E123" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F123" t="s">
-        <v>183</v>
-      </c>
-      <c r="G123">
+      <c r="C136" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D136" t="s">
+        <v>198</v>
+      </c>
+      <c r="E136" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F136" t="s">
+        <v>201</v>
+      </c>
+      <c r="G136">
         <v>1.25</v>
       </c>
-      <c r="H123">
-        <v>1</v>
-      </c>
-      <c r="I123">
+      <c r="H136">
+        <v>1</v>
+      </c>
+      <c r="I136">
         <v>100</v>
       </c>
-      <c r="J123">
+      <c r="J136">
         <f t="shared" si="1"/>
         <v>125</v>
       </c>
-      <c r="K123" t="s">
+      <c r="K136" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="124" spans="1:11">
-      <c r="A124" s="1">
+    <row r="137" spans="1:11">
+      <c r="A137" s="1">
         <v>44365</v>
       </c>
-      <c r="B124" s="1">
+      <c r="B137" s="1">
         <v>44365</v>
       </c>
-      <c r="C124" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D124" t="s">
-        <v>184</v>
-      </c>
-      <c r="E124" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F124" s="3" t="s">
+      <c r="C137" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D137" t="s">
+        <v>202</v>
+      </c>
+      <c r="E137" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F137" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G124">
+      <c r="G137">
         <v>1.65</v>
       </c>
-      <c r="H124">
-        <v>0</v>
-      </c>
-      <c r="I124">
+      <c r="H137">
+        <v>0</v>
+      </c>
+      <c r="I137">
         <v>50</v>
       </c>
-      <c r="J124">
-        <v>0</v>
-      </c>
-      <c r="K124" t="s">
+      <c r="J137">
+        <v>0</v>
+      </c>
+      <c r="K137" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="125" spans="1:11">
-      <c r="A125" s="1">
+    <row r="138" spans="1:11">
+      <c r="A138" s="1">
         <v>44365</v>
       </c>
-      <c r="B125" s="1">
+      <c r="B138" s="1">
         <v>44365</v>
       </c>
-      <c r="C125" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D125" t="s">
-        <v>184</v>
-      </c>
-      <c r="E125" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F125" t="s">
+      <c r="C138" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D138" t="s">
+        <v>202</v>
+      </c>
+      <c r="E138" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F138" t="s">
         <v>87</v>
       </c>
-      <c r="G125">
+      <c r="G138">
         <v>1.42</v>
       </c>
-      <c r="H125">
-        <v>1</v>
-      </c>
-      <c r="I125">
+      <c r="H138">
+        <v>1</v>
+      </c>
+      <c r="I138">
         <v>50</v>
       </c>
-      <c r="J125">
-        <f t="shared" ref="J125:J127" si="2">G125 * I125</f>
+      <c r="J138">
+        <f t="shared" ref="J138:J140" si="2">G138 * I138</f>
         <v>71</v>
       </c>
-      <c r="K125" t="s">
+      <c r="K138" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="126" spans="1:11">
-      <c r="A126" s="1">
+    <row r="139" spans="1:11">
+      <c r="A139" s="1">
         <v>44364</v>
       </c>
-      <c r="B126" s="1">
+      <c r="B139" s="1">
         <v>44364</v>
       </c>
-      <c r="C126" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D126" t="s">
-        <v>185</v>
-      </c>
-      <c r="E126" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F126" s="3" t="s">
+      <c r="C139" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D139" t="s">
+        <v>203</v>
+      </c>
+      <c r="E139" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F139" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G126">
+      <c r="G139">
         <v>1.1599999999999999</v>
       </c>
-      <c r="H126">
-        <v>1</v>
-      </c>
-      <c r="I126">
+      <c r="H139">
+        <v>1</v>
+      </c>
+      <c r="I139">
         <v>100</v>
       </c>
-      <c r="J126">
+      <c r="J139">
         <f t="shared" si="2"/>
         <v>115.99999999999999</v>
       </c>
-      <c r="K126" t="s">
+      <c r="K139" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="127" spans="1:11">
-      <c r="A127" s="1">
+    <row r="140" spans="1:11">
+      <c r="A140" s="1">
         <v>44364</v>
       </c>
-      <c r="B127" s="1">
+      <c r="B140" s="1">
         <v>44364</v>
       </c>
-      <c r="C127" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D127" t="s">
-        <v>186</v>
-      </c>
-      <c r="E127" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F127" s="3" t="s">
+      <c r="C140" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D140" t="s">
+        <v>204</v>
+      </c>
+      <c r="E140" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F140" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="G127">
+      <c r="G140">
         <v>1.18</v>
       </c>
-      <c r="H127">
-        <v>1</v>
-      </c>
-      <c r="I127">
+      <c r="H140">
+        <v>1</v>
+      </c>
+      <c r="I140">
         <v>100</v>
       </c>
-      <c r="J127">
+      <c r="J140">
         <f t="shared" si="2"/>
         <v>118</v>
       </c>
-      <c r="K127" t="s">
+      <c r="K140" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="128" spans="1:11">
-      <c r="A128" s="1">
+    <row r="141" spans="1:11">
+      <c r="A141" s="1">
         <v>44363</v>
       </c>
-      <c r="B128" s="1">
+      <c r="B141" s="1">
         <v>44363</v>
       </c>
-      <c r="C128" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D128" t="s">
-        <v>187</v>
-      </c>
-      <c r="E128" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F128" t="s">
-        <v>170</v>
-      </c>
-      <c r="G128">
+      <c r="C141" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D141" t="s">
+        <v>205</v>
+      </c>
+      <c r="E141" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F141" t="s">
+        <v>188</v>
+      </c>
+      <c r="G141">
         <v>1.4</v>
       </c>
-      <c r="H128">
-        <v>1</v>
-      </c>
-      <c r="I128">
+      <c r="H141">
+        <v>1</v>
+      </c>
+      <c r="I141">
         <v>100</v>
       </c>
-      <c r="J128">
-        <f t="shared" ref="J128:J129" si="3">G128 * I128</f>
+      <c r="J141">
+        <f t="shared" ref="J141:J142" si="3">G141 * I141</f>
         <v>140</v>
       </c>
-      <c r="K128" t="s">
+      <c r="K141" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="129" spans="1:11">
-      <c r="A129" s="1">
+    <row r="142" spans="1:11">
+      <c r="A142" s="1">
         <v>44363</v>
       </c>
-      <c r="B129" s="1">
+      <c r="B142" s="1">
         <v>44363</v>
       </c>
-      <c r="C129" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D129" t="s">
-        <v>187</v>
-      </c>
-      <c r="E129" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F129" s="3" t="s">
+      <c r="C142" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D142" t="s">
+        <v>205</v>
+      </c>
+      <c r="E142" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F142" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G129">
+      <c r="G142">
         <v>1.22</v>
       </c>
-      <c r="H129">
-        <v>1</v>
-      </c>
-      <c r="I129">
+      <c r="H142">
+        <v>1</v>
+      </c>
+      <c r="I142">
         <v>100</v>
       </c>
-      <c r="J129">
+      <c r="J142">
         <f t="shared" si="3"/>
         <v>122</v>
       </c>
-      <c r="K129" t="s">
+      <c r="K142" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="130" spans="1:11">
-      <c r="A130" s="1">
+    <row r="143" spans="1:11">
+      <c r="A143" s="1">
         <v>44362</v>
       </c>
-      <c r="B130" s="1">
+      <c r="B143" s="1">
         <v>44362</v>
       </c>
-      <c r="C130" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D130" t="s">
-        <v>188</v>
-      </c>
-      <c r="E130" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F130" t="s">
+      <c r="C143" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D143" t="s">
+        <v>206</v>
+      </c>
+      <c r="E143" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F143" t="s">
         <v>87</v>
       </c>
-      <c r="G130">
+      <c r="G143">
         <v>1.77</v>
       </c>
-      <c r="H130">
-        <v>0</v>
-      </c>
-      <c r="I130">
+      <c r="H143">
+        <v>0</v>
+      </c>
+      <c r="I143">
         <v>100</v>
       </c>
-      <c r="J130">
-        <v>0</v>
-      </c>
-      <c r="K130" t="s">
+      <c r="J143">
+        <v>0</v>
+      </c>
+      <c r="K143" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="131" spans="1:11">
-      <c r="A131" s="1">
+    <row r="144" spans="1:11">
+      <c r="A144" s="1">
         <v>44361</v>
       </c>
-      <c r="B131" s="1">
+      <c r="B144" s="1">
         <v>44361</v>
       </c>
-      <c r="C131" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D131" t="s">
-        <v>189</v>
-      </c>
-      <c r="E131" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="F131" t="s">
-        <v>190</v>
-      </c>
-      <c r="G131">
+      <c r="C144" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D144" t="s">
+        <v>207</v>
+      </c>
+      <c r="E144" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F144" t="s">
+        <v>208</v>
+      </c>
+      <c r="G144">
         <v>1.27</v>
       </c>
-      <c r="H131">
-        <v>0</v>
-      </c>
-      <c r="I131">
+      <c r="H144">
+        <v>0</v>
+      </c>
+      <c r="I144">
         <v>100</v>
       </c>
-      <c r="J131">
-        <v>0</v>
-      </c>
-      <c r="K131" t="s">
+      <c r="J144">
+        <v>0</v>
+      </c>
+      <c r="K144" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="132" spans="1:11">
-      <c r="A132" s="1">
+    <row r="145" spans="1:11">
+      <c r="A145" s="1">
         <v>44359</v>
       </c>
-      <c r="B132" s="1">
+      <c r="B145" s="1">
         <v>44359</v>
       </c>
-      <c r="C132" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D132" t="s">
-        <v>191</v>
-      </c>
-      <c r="E132" t="s">
-        <v>12</v>
-      </c>
-      <c r="F132" t="s">
+      <c r="C145" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D145" t="s">
+        <v>209</v>
+      </c>
+      <c r="E145" t="s">
+        <v>12</v>
+      </c>
+      <c r="F145" t="s">
         <v>106</v>
       </c>
-      <c r="G132">
+      <c r="G145">
         <v>3.9</v>
       </c>
-      <c r="H132">
-        <v>0</v>
-      </c>
-      <c r="I132">
-        <v>0</v>
-      </c>
-      <c r="J132">
-        <f t="shared" ref="J131:J133" si="4">G132 * I132</f>
-        <v>0</v>
-      </c>
-      <c r="K132" t="s">
+      <c r="H145">
+        <v>0</v>
+      </c>
+      <c r="I145">
+        <v>0</v>
+      </c>
+      <c r="J145">
+        <f t="shared" ref="J144:J146" si="4">G145 * I145</f>
+        <v>0</v>
+      </c>
+      <c r="K145" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="133" spans="1:11">
-      <c r="A133" s="1">
+    <row r="146" spans="1:11">
+      <c r="A146" s="1">
         <v>44358</v>
       </c>
-      <c r="B133" s="1">
+      <c r="B146" s="1">
         <v>44358</v>
       </c>
-      <c r="C133" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D133" t="s">
-        <v>192</v>
-      </c>
-      <c r="E133" t="s">
-        <v>32</v>
-      </c>
-      <c r="F133" t="s">
-        <v>193</v>
-      </c>
-      <c r="G133">
+      <c r="C146" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D146" t="s">
+        <v>210</v>
+      </c>
+      <c r="E146" t="s">
+        <v>32</v>
+      </c>
+      <c r="F146" t="s">
+        <v>211</v>
+      </c>
+      <c r="G146">
         <v>1.17</v>
       </c>
-      <c r="H133">
-        <v>1</v>
-      </c>
-      <c r="I133">
+      <c r="H146">
+        <v>1</v>
+      </c>
+      <c r="I146">
         <v>50</v>
       </c>
-      <c r="J133">
+      <c r="J146">
         <f t="shared" si="4"/>
         <v>58.5</v>
       </c>
-      <c r="K133" t="s">
+      <c r="K146" t="s">
         <v>34</v>
-      </c>
-    </row>
-    <row r="134" spans="1:11">
-      <c r="A134" s="1">
-        <v>44358</v>
-      </c>
-      <c r="B134" s="1">
-        <v>44358</v>
-      </c>
-      <c r="C134" s="2" t="s">
-        <v>176</v>
-      </c>
-      <c r="D134" t="s">
-        <v>192</v>
-      </c>
-      <c r="E134" t="s">
-        <v>32</v>
-      </c>
-      <c r="F134" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G134">
-        <v>1.0900000000000001</v>
-      </c>
-      <c r="H134">
-        <v>1</v>
-      </c>
-      <c r="I134">
-        <v>100</v>
-      </c>
-      <c r="J134">
-        <f>G134 * I134</f>
-        <v>109.00000000000001</v>
-      </c>
-      <c r="K134" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="135" spans="1:11">
-      <c r="A135" s="1">
-        <v>44339</v>
-      </c>
-      <c r="B135" s="1">
-        <v>44339</v>
-      </c>
-      <c r="C135" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D135" t="s">
-        <v>194</v>
-      </c>
-      <c r="E135" t="s">
-        <v>32</v>
-      </c>
-      <c r="F135" t="s">
-        <v>195</v>
-      </c>
-      <c r="G135">
-        <v>1.18</v>
-      </c>
-      <c r="H135">
-        <v>1</v>
-      </c>
-      <c r="I135">
-        <v>50</v>
-      </c>
-      <c r="J135">
-        <f>G135 * I135</f>
-        <v>59</v>
-      </c>
-      <c r="K135" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="136" spans="1:11">
-      <c r="A136" s="1">
-        <v>44339</v>
-      </c>
-      <c r="B136" s="1">
-        <v>44339</v>
-      </c>
-      <c r="C136" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D136" t="s">
-        <v>194</v>
-      </c>
-      <c r="E136" t="s">
-        <v>32</v>
-      </c>
-      <c r="F136" t="s">
-        <v>96</v>
-      </c>
-      <c r="G136">
-        <v>1.1499999999999999</v>
-      </c>
-      <c r="H136">
-        <v>1</v>
-      </c>
-      <c r="I136">
-        <v>100</v>
-      </c>
-      <c r="J136">
-        <f>G136 * I136</f>
-        <v>114.99999999999999</v>
-      </c>
-      <c r="K136" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="137" spans="1:11">
-      <c r="A137" s="1">
-        <v>44335</v>
-      </c>
-      <c r="B137" s="1">
-        <v>44335</v>
-      </c>
-      <c r="C137" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D137" t="s">
-        <v>196</v>
-      </c>
-      <c r="E137" t="s">
-        <v>32</v>
-      </c>
-      <c r="F137" t="s">
-        <v>97</v>
-      </c>
-      <c r="G137">
-        <v>2.2000000000000002</v>
-      </c>
-      <c r="H137">
-        <v>1</v>
-      </c>
-      <c r="I137">
-        <v>25</v>
-      </c>
-      <c r="J137">
-        <f>G137 * I137</f>
-        <v>55.000000000000007</v>
-      </c>
-      <c r="K137" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="138" spans="1:11">
-      <c r="A138" s="1">
-        <v>44332</v>
-      </c>
-      <c r="B138" s="1">
-        <v>44332</v>
-      </c>
-      <c r="C138" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D138" t="s">
-        <v>197</v>
-      </c>
-      <c r="E138" t="s">
-        <v>32</v>
-      </c>
-      <c r="F138" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G138">
-        <v>1.27</v>
-      </c>
-      <c r="H138">
-        <v>1</v>
-      </c>
-      <c r="I138">
-        <v>25</v>
-      </c>
-      <c r="J138">
-        <f>G138 * I138</f>
-        <v>31.75</v>
-      </c>
-      <c r="K138" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="139" spans="1:11">
-      <c r="A139" s="1">
-        <v>44329</v>
-      </c>
-      <c r="B139" s="1">
-        <v>44329</v>
-      </c>
-      <c r="C139" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D139" t="s">
-        <v>150</v>
-      </c>
-      <c r="E139" t="s">
-        <v>12</v>
-      </c>
-      <c r="F139" t="s">
-        <v>198</v>
-      </c>
-      <c r="G139">
-        <v>1.6</v>
-      </c>
-      <c r="H139">
-        <v>1</v>
-      </c>
-      <c r="I139">
-        <v>10</v>
-      </c>
-      <c r="J139">
-        <f>G139 * I139</f>
-        <v>16</v>
-      </c>
-      <c r="K139" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="140" spans="1:11">
-      <c r="A140" s="1">
-        <v>44329</v>
-      </c>
-      <c r="B140" s="1">
-        <v>44329</v>
-      </c>
-      <c r="C140" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D140" t="s">
-        <v>150</v>
-      </c>
-      <c r="E140" t="s">
-        <v>12</v>
-      </c>
-      <c r="F140" t="s">
-        <v>106</v>
-      </c>
-      <c r="G140">
-        <v>3.65</v>
-      </c>
-      <c r="H140">
-        <v>0</v>
-      </c>
-      <c r="I140">
-        <v>10</v>
-      </c>
-      <c r="J140">
-        <v>0</v>
-      </c>
-      <c r="K140" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="141" spans="1:11">
-      <c r="A141" s="1">
-        <v>44305</v>
-      </c>
-      <c r="B141" s="1">
-        <v>44305</v>
-      </c>
-      <c r="C141" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D141" t="s">
-        <v>166</v>
-      </c>
-      <c r="E141" t="s">
-        <v>32</v>
-      </c>
-      <c r="F141" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="G141">
-        <v>1.52</v>
-      </c>
-      <c r="H141">
-        <v>0</v>
-      </c>
-      <c r="I141">
-        <v>100</v>
-      </c>
-      <c r="J141">
-        <f>G141 * I141</f>
-        <v>152</v>
-      </c>
-      <c r="K141" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="142" spans="1:11">
-      <c r="A142" s="1">
-        <v>44292</v>
-      </c>
-      <c r="B142" s="1">
-        <v>44292</v>
-      </c>
-      <c r="C142" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D142" t="s">
-        <v>199</v>
-      </c>
-      <c r="E142" t="s">
-        <v>32</v>
-      </c>
-      <c r="F142" t="s">
-        <v>200</v>
-      </c>
-      <c r="G142">
-        <v>1.1000000000000001</v>
-      </c>
-      <c r="H142">
-        <v>0</v>
-      </c>
-      <c r="I142">
-        <v>100</v>
-      </c>
-      <c r="J142">
-        <v>0</v>
-      </c>
-      <c r="K142" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="143" spans="1:11">
-      <c r="A143" s="1">
-        <v>44292</v>
-      </c>
-      <c r="B143" s="1">
-        <v>44292</v>
-      </c>
-      <c r="C143" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D143" t="s">
-        <v>199</v>
-      </c>
-      <c r="E143" t="s">
-        <v>12</v>
-      </c>
-      <c r="F143" t="s">
-        <v>87</v>
-      </c>
-      <c r="G143">
-        <v>2.15</v>
-      </c>
-      <c r="H143">
-        <v>0</v>
-      </c>
-      <c r="I143">
-        <v>50</v>
-      </c>
-      <c r="J143">
-        <v>0</v>
-      </c>
-      <c r="K143" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="144" spans="1:11">
-      <c r="A144" s="1">
-        <v>44292</v>
-      </c>
-      <c r="B144" s="1">
-        <v>44292</v>
-      </c>
-      <c r="C144" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="D144" t="s">
-        <v>199</v>
-      </c>
-      <c r="E144" t="s">
-        <v>12</v>
-      </c>
-      <c r="F144" t="s">
-        <v>159</v>
-      </c>
-      <c r="G144">
-        <v>1.33</v>
-      </c>
-      <c r="H144">
-        <v>1</v>
-      </c>
-      <c r="I144">
-        <v>45</v>
-      </c>
-      <c r="J144">
-        <f>G144 * I144</f>
-        <v>59.85</v>
-      </c>
-      <c r="K144" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="145" spans="1:11">
-      <c r="A145" s="1">
-        <v>44290</v>
-      </c>
-      <c r="B145" s="1">
-        <v>44290</v>
-      </c>
-      <c r="C145" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D145" t="s">
-        <v>201</v>
-      </c>
-      <c r="E145" t="s">
-        <v>32</v>
-      </c>
-      <c r="F145" t="s">
-        <v>202</v>
-      </c>
-      <c r="G145">
-        <v>1.6</v>
-      </c>
-      <c r="H145">
-        <v>0</v>
-      </c>
-      <c r="I145">
-        <v>100</v>
-      </c>
-      <c r="J145">
-        <v>0</v>
-      </c>
-      <c r="K145" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="146" spans="1:11">
-      <c r="A146" s="1">
-        <v>44290</v>
-      </c>
-      <c r="B146" s="1">
-        <v>44290</v>
-      </c>
-      <c r="C146" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D146" t="s">
-        <v>201</v>
-      </c>
-      <c r="E146" t="s">
-        <v>32</v>
-      </c>
-      <c r="F146" t="s">
-        <v>203</v>
-      </c>
-      <c r="G146">
-        <v>1.28</v>
-      </c>
-      <c r="H146">
-        <v>1</v>
-      </c>
-      <c r="I146">
-        <v>100</v>
-      </c>
-      <c r="J146">
-        <f>G146 * I146</f>
-        <v>128</v>
-      </c>
-      <c r="K146" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="147" spans="1:11">
       <c r="A147" s="1">
-        <v>44290</v>
+        <v>44358</v>
       </c>
       <c r="B147" s="1">
-        <v>44290</v>
+        <v>44358</v>
       </c>
       <c r="C147" s="2" t="s">
-        <v>11</v>
+        <v>194</v>
       </c>
       <c r="D147" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
       <c r="E147" t="s">
         <v>32</v>
@@ -6185,16 +6232,17 @@
         <v>53</v>
       </c>
       <c r="G147">
-        <v>1.97</v>
+        <v>1.0900000000000001</v>
       </c>
       <c r="H147">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I147">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J147">
-        <v>14.62</v>
+        <f>G147 * I147</f>
+        <v>109.00000000000001</v>
       </c>
       <c r="K147" t="s">
         <v>17</v>
@@ -6202,25 +6250,25 @@
     </row>
     <row r="148" spans="1:11">
       <c r="A148" s="1">
-        <v>44289</v>
+        <v>44339</v>
       </c>
       <c r="B148" s="1">
-        <v>44289</v>
+        <v>44339</v>
       </c>
       <c r="C148" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D148" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
       <c r="E148" t="s">
         <v>32</v>
       </c>
       <c r="F148" t="s">
-        <v>83</v>
+        <v>213</v>
       </c>
       <c r="G148">
-        <v>4.8</v>
+        <v>1.18</v>
       </c>
       <c r="H148">
         <v>1</v>
@@ -6230,59 +6278,523 @@
       </c>
       <c r="J148">
         <f>G148 * I148</f>
-        <v>240</v>
+        <v>59</v>
       </c>
       <c r="K148" t="s">
-        <v>84</v>
+        <v>55</v>
       </c>
     </row>
     <row r="149" spans="1:11">
       <c r="A149" s="1">
-        <v>44289</v>
+        <v>44339</v>
       </c>
       <c r="B149" s="1">
-        <v>44289</v>
+        <v>44339</v>
       </c>
       <c r="C149" s="2" t="s">
         <v>11</v>
       </c>
       <c r="D149" t="s">
-        <v>128</v>
+        <v>212</v>
       </c>
       <c r="E149" t="s">
         <v>32</v>
       </c>
       <c r="F149" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="G149">
-        <v>2.2000000000000002</v>
+        <v>1.1499999999999999</v>
       </c>
       <c r="H149">
         <v>1</v>
       </c>
       <c r="I149">
-        <v>50</v>
+        <v>100</v>
       </c>
       <c r="J149">
         <f>G149 * I149</f>
+        <v>114.99999999999999</v>
+      </c>
+      <c r="K149" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="150" spans="1:11">
+      <c r="A150" s="1">
+        <v>44335</v>
+      </c>
+      <c r="B150" s="1">
+        <v>44335</v>
+      </c>
+      <c r="C150" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D150" t="s">
+        <v>214</v>
+      </c>
+      <c r="E150" t="s">
+        <v>32</v>
+      </c>
+      <c r="F150" t="s">
+        <v>97</v>
+      </c>
+      <c r="G150">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H150">
+        <v>1</v>
+      </c>
+      <c r="I150">
+        <v>25</v>
+      </c>
+      <c r="J150">
+        <f>G150 * I150</f>
+        <v>55.000000000000007</v>
+      </c>
+      <c r="K150" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="151" spans="1:11">
+      <c r="A151" s="1">
+        <v>44332</v>
+      </c>
+      <c r="B151" s="1">
+        <v>44332</v>
+      </c>
+      <c r="C151" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D151" t="s">
+        <v>215</v>
+      </c>
+      <c r="E151" t="s">
+        <v>32</v>
+      </c>
+      <c r="F151" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G151">
+        <v>1.27</v>
+      </c>
+      <c r="H151">
+        <v>1</v>
+      </c>
+      <c r="I151">
+        <v>25</v>
+      </c>
+      <c r="J151">
+        <f>G151 * I151</f>
+        <v>31.75</v>
+      </c>
+      <c r="K151" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="152" spans="1:11">
+      <c r="A152" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B152" s="1">
+        <v>44329</v>
+      </c>
+      <c r="C152" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D152" t="s">
+        <v>168</v>
+      </c>
+      <c r="E152" t="s">
+        <v>12</v>
+      </c>
+      <c r="F152" t="s">
+        <v>216</v>
+      </c>
+      <c r="G152">
+        <v>1.6</v>
+      </c>
+      <c r="H152">
+        <v>1</v>
+      </c>
+      <c r="I152">
+        <v>10</v>
+      </c>
+      <c r="J152">
+        <f>G152 * I152</f>
+        <v>16</v>
+      </c>
+      <c r="K152" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="153" spans="1:11">
+      <c r="A153" s="1">
+        <v>44329</v>
+      </c>
+      <c r="B153" s="1">
+        <v>44329</v>
+      </c>
+      <c r="C153" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D153" t="s">
+        <v>168</v>
+      </c>
+      <c r="E153" t="s">
+        <v>12</v>
+      </c>
+      <c r="F153" t="s">
+        <v>106</v>
+      </c>
+      <c r="G153">
+        <v>3.65</v>
+      </c>
+      <c r="H153">
+        <v>0</v>
+      </c>
+      <c r="I153">
+        <v>10</v>
+      </c>
+      <c r="J153">
+        <v>0</v>
+      </c>
+      <c r="K153" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="154" spans="1:11">
+      <c r="A154" s="1">
+        <v>44305</v>
+      </c>
+      <c r="B154" s="1">
+        <v>44305</v>
+      </c>
+      <c r="C154" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D154" t="s">
+        <v>184</v>
+      </c>
+      <c r="E154" t="s">
+        <v>32</v>
+      </c>
+      <c r="F154" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G154">
+        <v>1.52</v>
+      </c>
+      <c r="H154">
+        <v>0</v>
+      </c>
+      <c r="I154">
+        <v>100</v>
+      </c>
+      <c r="J154">
+        <f>G154 * I154</f>
+        <v>152</v>
+      </c>
+      <c r="K154" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="155" spans="1:11">
+      <c r="A155" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B155" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C155" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D155" t="s">
+        <v>217</v>
+      </c>
+      <c r="E155" t="s">
+        <v>32</v>
+      </c>
+      <c r="F155" t="s">
+        <v>218</v>
+      </c>
+      <c r="G155">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="H155">
+        <v>0</v>
+      </c>
+      <c r="I155">
+        <v>100</v>
+      </c>
+      <c r="J155">
+        <v>0</v>
+      </c>
+      <c r="K155" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="156" spans="1:11">
+      <c r="A156" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B156" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C156" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D156" t="s">
+        <v>217</v>
+      </c>
+      <c r="E156" t="s">
+        <v>12</v>
+      </c>
+      <c r="F156" t="s">
+        <v>87</v>
+      </c>
+      <c r="G156">
+        <v>2.15</v>
+      </c>
+      <c r="H156">
+        <v>0</v>
+      </c>
+      <c r="I156">
+        <v>50</v>
+      </c>
+      <c r="J156">
+        <v>0</v>
+      </c>
+      <c r="K156" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="157" spans="1:11">
+      <c r="A157" s="1">
+        <v>44292</v>
+      </c>
+      <c r="B157" s="1">
+        <v>44292</v>
+      </c>
+      <c r="C157" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="D157" t="s">
+        <v>217</v>
+      </c>
+      <c r="E157" t="s">
+        <v>12</v>
+      </c>
+      <c r="F157" t="s">
+        <v>177</v>
+      </c>
+      <c r="G157">
+        <v>1.33</v>
+      </c>
+      <c r="H157">
+        <v>1</v>
+      </c>
+      <c r="I157">
+        <v>45</v>
+      </c>
+      <c r="J157">
+        <f>G157 * I157</f>
+        <v>59.85</v>
+      </c>
+      <c r="K157" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="158" spans="1:11">
+      <c r="A158" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B158" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C158" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D158" t="s">
+        <v>219</v>
+      </c>
+      <c r="E158" t="s">
+        <v>32</v>
+      </c>
+      <c r="F158" t="s">
+        <v>220</v>
+      </c>
+      <c r="G158">
+        <v>1.6</v>
+      </c>
+      <c r="H158">
+        <v>0</v>
+      </c>
+      <c r="I158">
+        <v>100</v>
+      </c>
+      <c r="J158">
+        <v>0</v>
+      </c>
+      <c r="K158" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="159" spans="1:11">
+      <c r="A159" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B159" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C159" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D159" t="s">
+        <v>219</v>
+      </c>
+      <c r="E159" t="s">
+        <v>32</v>
+      </c>
+      <c r="F159" t="s">
+        <v>221</v>
+      </c>
+      <c r="G159">
+        <v>1.28</v>
+      </c>
+      <c r="H159">
+        <v>1</v>
+      </c>
+      <c r="I159">
+        <v>100</v>
+      </c>
+      <c r="J159">
+        <f>G159 * I159</f>
+        <v>128</v>
+      </c>
+      <c r="K159" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="160" spans="1:11">
+      <c r="A160" s="1">
+        <v>44290</v>
+      </c>
+      <c r="B160" s="1">
+        <v>44290</v>
+      </c>
+      <c r="C160" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D160" t="s">
+        <v>219</v>
+      </c>
+      <c r="E160" t="s">
+        <v>32</v>
+      </c>
+      <c r="F160" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G160">
+        <v>1.97</v>
+      </c>
+      <c r="H160">
+        <v>0</v>
+      </c>
+      <c r="I160">
+        <v>50</v>
+      </c>
+      <c r="J160">
+        <v>14.62</v>
+      </c>
+      <c r="K160" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="161" spans="1:11">
+      <c r="A161" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B161" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C161" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D161" t="s">
+        <v>128</v>
+      </c>
+      <c r="E161" t="s">
+        <v>32</v>
+      </c>
+      <c r="F161" t="s">
+        <v>83</v>
+      </c>
+      <c r="G161">
+        <v>4.8</v>
+      </c>
+      <c r="H161">
+        <v>1</v>
+      </c>
+      <c r="I161">
+        <v>50</v>
+      </c>
+      <c r="J161">
+        <f>G161 * I161</f>
+        <v>240</v>
+      </c>
+      <c r="K161" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="162" spans="1:11">
+      <c r="A162" s="1">
+        <v>44289</v>
+      </c>
+      <c r="B162" s="1">
+        <v>44289</v>
+      </c>
+      <c r="C162" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D162" t="s">
+        <v>128</v>
+      </c>
+      <c r="E162" t="s">
+        <v>32</v>
+      </c>
+      <c r="F162" t="s">
+        <v>87</v>
+      </c>
+      <c r="G162">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="H162">
+        <v>1</v>
+      </c>
+      <c r="I162">
+        <v>50</v>
+      </c>
+      <c r="J162">
+        <f>G162 * I162</f>
         <v>110.00000000000001</v>
       </c>
-      <c r="K149" t="s">
+      <c r="K162" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:K1" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54586E09-9FFB-4E9E-9508-271C90B80E05}">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -6292,36 +6804,29 @@
     <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
-        <v>204</v>
-      </c>
-      <c r="B1" t="s">
-        <v>205</v>
-      </c>
-      <c r="C1" t="s">
-        <v>206</v>
-      </c>
-      <c r="D1" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4">
-      <c r="A2" s="4">
-        <f xml:space="preserve"> SUM(Odds!J:J)</f>
-        <v>6198.9174000000003</v>
-      </c>
-      <c r="B2">
-        <f xml:space="preserve"> SUM(Odds!I:I)</f>
-        <v>6733.22</v>
-      </c>
-      <c r="C2">
-        <f>A2 - B2</f>
-        <v>-534.30259999999998</v>
-      </c>
-      <c r="D2">
-        <f>ROUND(100 * (C2 / B2), 2)</f>
-        <v>-7.94</v>
+        <v>222</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>